<commit_message>
Rename sheets and format pivot tables
</commit_message>
<xml_diff>
--- a/bike-sales.xlsx
+++ b/bike-sales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects Data Analyst\Excel Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD16F5B-DA1E-4799-B5D3-F11D617341F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F03E2DE-48AC-4836-8D72-A80A1E57BC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Sheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -197,8 +197,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -699,20 +699,19 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -761,75 +760,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -858,7 +791,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Excel Project Dataset.xlsx]Pivot Table!PivotTable1</c:name>
+    <c:name>[bike-sales.xlsx]Pivot Table!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -950,27 +883,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="63500">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="25000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1033,27 +946,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="63500">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="25000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1659,7 +1552,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Excel Project Dataset.xlsx]Pivot Table!PivotTable2</c:name>
+    <c:name>[bike-sales.xlsx]Pivot Table!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1853,7 +1746,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$B$24:$B$25</c:f>
+              <c:f>'Pivot Table'!$K$1:$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1876,7 +1769,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$26:$A$31</c:f>
+              <c:f>'Pivot Table'!$J$3:$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1899,7 +1792,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$B$26:$B$31</c:f>
+              <c:f>'Pivot Table'!$K$3:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1933,7 +1826,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$C$24:$C$25</c:f>
+              <c:f>'Pivot Table'!$L$1:$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1956,7 +1849,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$26:$A$31</c:f>
+              <c:f>'Pivot Table'!$J$3:$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1979,7 +1872,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$C$26:$C$31</c:f>
+              <c:f>'Pivot Table'!$L$3:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2297,7 +2190,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Excel Project Dataset.xlsx]Pivot Table!PivotTable3</c:name>
+    <c:name>[bike-sales.xlsx]Pivot Table!PivotTable3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2510,7 +2403,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$B$45:$B$46</c:f>
+              <c:f>'Pivot Table'!$E$28:$E$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2545,7 +2438,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$47:$A$50</c:f>
+              <c:f>'Pivot Table'!$D$30:$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2562,7 +2455,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$B$47:$B$50</c:f>
+              <c:f>'Pivot Table'!$E$30:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2590,7 +2483,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$C$45:$C$46</c:f>
+              <c:f>'Pivot Table'!$F$28:$F$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2625,7 +2518,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$47:$A$50</c:f>
+              <c:f>'Pivot Table'!$D$30:$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2642,7 +2535,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$C$47:$C$50</c:f>
+              <c:f>'Pivot Table'!$F$30:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2955,7 +2848,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Excel Project Dataset.xlsx]Pivot Table!PivotTable1</c:name>
+    <c:name>[bike-sales.xlsx]Pivot Table!PivotTable1</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -4008,7 +3901,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Excel Project Dataset.xlsx]Pivot Table!PivotTable2</c:name>
+    <c:name>[bike-sales.xlsx]Pivot Table!PivotTable2</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -4446,7 +4339,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$B$24:$B$25</c:f>
+              <c:f>'Pivot Table'!$K$1:$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4469,7 +4362,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$26:$A$31</c:f>
+              <c:f>'Pivot Table'!$J$3:$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4492,7 +4385,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$B$26:$B$31</c:f>
+              <c:f>'Pivot Table'!$K$3:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4526,7 +4419,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$C$24:$C$25</c:f>
+              <c:f>'Pivot Table'!$L$1:$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4549,7 +4442,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$26:$A$31</c:f>
+              <c:f>'Pivot Table'!$J$3:$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4572,7 +4465,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$C$26:$C$31</c:f>
+              <c:f>'Pivot Table'!$L$3:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4890,7 +4783,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Excel Project Dataset.xlsx]Pivot Table!PivotTable3</c:name>
+    <c:name>[bike-sales.xlsx]Pivot Table!PivotTable3</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -5387,7 +5280,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$B$45:$B$46</c:f>
+              <c:f>'Pivot Table'!$E$28:$E$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5422,7 +5315,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$47:$A$50</c:f>
+              <c:f>'Pivot Table'!$D$30:$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -5439,7 +5332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$B$47:$B$50</c:f>
+              <c:f>'Pivot Table'!$E$30:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -5467,7 +5360,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot Table'!$C$45:$C$46</c:f>
+              <c:f>'Pivot Table'!$F$28:$F$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5502,7 +5395,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Pivot Table'!$A$47:$A$50</c:f>
+              <c:f>'Pivot Table'!$D$30:$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -5519,7 +5412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot Table'!$C$47:$C$50</c:f>
+              <c:f>'Pivot Table'!$F$30:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -9198,16 +9091,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9234,16 +9127,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>11430</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9270,16 +9163,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9436,8 +9329,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Marital Status">
@@ -9460,7 +9353,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -9514,8 +9407,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>45721</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="6" name="Education">
@@ -9538,7 +9431,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -9592,8 +9485,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="Region">
@@ -9616,7 +9509,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -9681,7 +9574,7 @@
         <s v="Male"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Income" numFmtId="165">
+    <cacheField name="Income" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10000" maxValue="170000"/>
     </cacheField>
     <cacheField name="Children" numFmtId="0">
@@ -25807,8 +25700,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DD01C27A-9F82-49C8-9534-7173BC44F670}" name="PivotTable4" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A66:D90" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0303CCE6-FEF4-49B3-89BD-71A3B9E5FB6E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="J1:M8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -25819,7 +25712,317 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="13"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="13" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09531715-9BA2-4DE1-A4C6-84E3BC5598C5}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A1:D5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item h="1" x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="13"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DD01C27A-9F82-49C8-9534-7173BC44F670}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="D52:G76" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item h="1" x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="6">
@@ -26046,9 +26249,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4E95075-11F4-413E-9855-B9E80086ED7D}" name="PivotTable3" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A45:D50" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4E95075-11F4-413E-9855-B9E80086ED7D}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="D28:G33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -26059,7 +26262,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="6">
@@ -26134,316 +26337,6 @@
   <dataFields count="1">
     <dataField name="Count of Purchased Bike" fld="13" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0303CCE6-FEF4-49B3-89BD-71A3B9E5FB6E}" name="PivotTable2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A24:D31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="4"/>
-        <item x="2"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="9"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="13"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="13" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="13" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09531715-9BA2-4DE1-A4C6-84E3BC5598C5}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A1:D5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="165" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="4"/>
-        <item x="2"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="13"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="2" baseItem="0" numFmtId="170"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="12">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
   <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
@@ -26874,15 +26767,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A931" workbookViewId="0">
-      <selection activeCell="J931" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.44140625" customWidth="1"/>
   </cols>
@@ -71939,30 +71833,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EB1302-45D1-468E-8D97-458B7FB9581D}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="J1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
@@ -71974,534 +71881,498 @@
       <c r="D2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="J2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>33000</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>26363.636363636364</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>29523.809523809523</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>36363.63636363636</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>34000</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>35625</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="J4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>34761.904761904763</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>28750</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>32162.162162162163</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="J5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8">
+        <v>21</v>
+      </c>
+      <c r="L8">
+        <v>16</v>
+      </c>
+      <c r="M8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31">
+        <v>11</v>
+      </c>
+      <c r="F31">
         <v>16</v>
       </c>
-      <c r="B26" s="3">
-        <v>5</v>
-      </c>
-      <c r="C26" s="3">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3">
-        <v>4</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3">
-        <v>8</v>
-      </c>
-      <c r="C28" s="3">
-        <v>5</v>
-      </c>
-      <c r="D28" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3">
+      <c r="G31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33">
+        <v>21</v>
+      </c>
+      <c r="F33">
+        <v>16</v>
+      </c>
+      <c r="G33">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D52" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D53" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D54" s="4">
+        <v>27</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D55" s="4">
+        <v>28</v>
+      </c>
+      <c r="E55">
         <v>3</v>
       </c>
-      <c r="C29" s="3">
+      <c r="G55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D56" s="4">
+        <v>29</v>
+      </c>
+      <c r="E56">
         <v>2</v>
       </c>
-      <c r="D29" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="G56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D57" s="4">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D58" s="4">
+        <v>31</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D59" s="4">
+        <v>32</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D60" s="4">
+        <v>33</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D61" s="4">
+        <v>34</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D62" s="4">
+        <v>35</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D63" s="4">
+        <v>36</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D64" s="4">
+        <v>37</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D65" s="4">
+        <v>38</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D66" s="4">
+        <v>39</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D67" s="4">
+        <v>40</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D68" s="4">
         <v>42</v>
       </c>
-      <c r="B30" s="3">
+      <c r="E68">
         <v>1</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3">
+      <c r="F68">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="G68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D69" s="4">
+        <v>43</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D70" s="4">
+        <v>45</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D71" s="4">
+        <v>46</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D72" s="4">
+        <v>50</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D73" s="4">
+        <v>51</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D74" s="4">
+        <v>56</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D75" s="4">
+        <v>57</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D76" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="3">
+      <c r="E76">
         <v>21</v>
       </c>
-      <c r="C31" s="3">
+      <c r="F76">
         <v>16</v>
       </c>
-      <c r="D31" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="3">
-        <v>8</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="3">
-        <v>11</v>
-      </c>
-      <c r="C48" s="3">
-        <v>16</v>
-      </c>
-      <c r="D48" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" s="3">
-        <v>2</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="3">
-        <v>21</v>
-      </c>
-      <c r="C50" s="3">
-        <v>16</v>
-      </c>
-      <c r="D50" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B67" t="s">
-        <v>18</v>
-      </c>
-      <c r="C67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="5">
-        <v>27</v>
-      </c>
-      <c r="B68" s="3">
-        <v>1</v>
-      </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="5">
-        <v>28</v>
-      </c>
-      <c r="B69" s="3">
-        <v>3</v>
-      </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="5">
-        <v>29</v>
-      </c>
-      <c r="B70" s="3">
-        <v>2</v>
-      </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="5">
-        <v>30</v>
-      </c>
-      <c r="B71" s="3">
-        <v>2</v>
-      </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="5">
-        <v>31</v>
-      </c>
-      <c r="B72" s="3">
-        <v>1</v>
-      </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="5">
-        <v>32</v>
-      </c>
-      <c r="B73" s="3">
-        <v>2</v>
-      </c>
-      <c r="C73" s="3">
-        <v>1</v>
-      </c>
-      <c r="D73" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="5">
-        <v>33</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3">
-        <v>1</v>
-      </c>
-      <c r="D74" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="5">
-        <v>34</v>
-      </c>
-      <c r="B75" s="3">
-        <v>1</v>
-      </c>
-      <c r="C75" s="3">
-        <v>2</v>
-      </c>
-      <c r="D75" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="5">
-        <v>35</v>
-      </c>
-      <c r="B76" s="3">
-        <v>2</v>
-      </c>
-      <c r="C76" s="3">
-        <v>1</v>
-      </c>
-      <c r="D76" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="5">
-        <v>36</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3">
-        <v>2</v>
-      </c>
-      <c r="D77" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="5">
-        <v>37</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3">
-        <v>1</v>
-      </c>
-      <c r="D78" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="5">
-        <v>38</v>
-      </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3">
-        <v>2</v>
-      </c>
-      <c r="D79" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="5">
-        <v>39</v>
-      </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3">
-        <v>1</v>
-      </c>
-      <c r="D80" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="5">
-        <v>40</v>
-      </c>
-      <c r="B81" s="3">
-        <v>1</v>
-      </c>
-      <c r="C81" s="3">
-        <v>1</v>
-      </c>
-      <c r="D81" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="5">
-        <v>42</v>
-      </c>
-      <c r="B82" s="3">
-        <v>1</v>
-      </c>
-      <c r="C82" s="3">
-        <v>1</v>
-      </c>
-      <c r="D82" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="5">
-        <v>43</v>
-      </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3">
-        <v>1</v>
-      </c>
-      <c r="D83" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="5">
-        <v>45</v>
-      </c>
-      <c r="B84" s="3">
-        <v>1</v>
-      </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="5">
-        <v>46</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3">
-        <v>1</v>
-      </c>
-      <c r="D85" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="5">
-        <v>50</v>
-      </c>
-      <c r="B86" s="3">
-        <v>1</v>
-      </c>
-      <c r="C86" s="3">
-        <v>1</v>
-      </c>
-      <c r="D86" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="5">
-        <v>51</v>
-      </c>
-      <c r="B87" s="3">
-        <v>1</v>
-      </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="5">
-        <v>56</v>
-      </c>
-      <c r="B88" s="3">
-        <v>1</v>
-      </c>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="5">
-        <v>57</v>
-      </c>
-      <c r="B89" s="3">
-        <v>1</v>
-      </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B90" s="3">
-        <v>21</v>
-      </c>
-      <c r="C90" s="3">
-        <v>16</v>
-      </c>
-      <c r="D90" s="3">
+      <c r="G76">
         <v>37</v>
       </c>
     </row>
@@ -72515,14 +72386,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFEF32-7163-4B11-9C4E-6BF8193F6BCA}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="7"/>

</xml_diff>